<commit_message>
sens.moveForward() #skiping slit     updateCposition()
</commit_message>
<xml_diff>
--- a/proxsens/pop.xlsx
+++ b/proxsens/pop.xlsx
@@ -21,6 +21,26 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>theta</t>
+  </si>
+  <si>
+    <t>pixel</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>Intercept</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -370,104 +390,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1">
-        <v>1.9599999999999999E-2</v>
-      </c>
-      <c r="B1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <f>ATAN2(C2,5)</f>
+        <v>3.0665230926948613E-2</v>
+      </c>
+      <c r="B2">
+        <v>8</v>
+      </c>
+      <c r="C2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <f t="shared" ref="A3:A9" si="0">ATAN2(C3,5)</f>
+        <v>3.495079653065275E-2</v>
+      </c>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <f t="shared" si="0"/>
+        <v>4.0628037681373123E-2</v>
+      </c>
+      <c r="B4">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4.8505612240383508E-2</v>
+      </c>
+      <c r="B5">
+        <v>18</v>
+      </c>
+      <c r="C5">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>2.23E-2</v>
-      </c>
-      <c r="B2">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>2.5600000000000001E-2</v>
-      </c>
-      <c r="B3">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>3.04E-2</v>
-      </c>
-      <c r="B4">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>3.7199999999999997E-2</v>
-      </c>
-      <c r="B5">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>4.7500000000000001E-2</v>
+        <f t="shared" si="0"/>
+        <v>6.0168251155009719E-2</v>
       </c>
       <c r="B6">
-        <v>131.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>6.6500000000000004E-2</v>
+        <f t="shared" si="0"/>
+        <v>7.9199070969451488E-2</v>
       </c>
       <c r="B7">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+        <v>35</v>
+      </c>
+      <c r="C7">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>0.1106</v>
+        <f t="shared" si="0"/>
+        <v>0.11575921772081071</v>
       </c>
       <c r="B8">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+        <v>50</v>
+      </c>
+      <c r="C8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>0.1651486774</v>
+        <f t="shared" si="0"/>
+        <v>0.21406068356382149</v>
       </c>
       <c r="B9">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>0.32169999999999999</v>
-      </c>
-      <c r="B10">
-        <v>429</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <f>SLOPE(A1:A10,B1:B10)</f>
-        <v>9.2348534554322341E-4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <f>INTERCEPT(A1:A10,B1:B10)</f>
-        <v>-7.4563240685107141E-2</v>
+        <f>SLOPE(A2:A9,B2:B9)</f>
+        <v>2.1261041696005799E-3</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <f>INTERCEPT(A2:A9,B2:B9)</f>
+        <v>9.6910161501378017E-3</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>